<commit_message>
Add varyingkscen2 and small changes to previous
</commit_message>
<xml_diff>
--- a/test/resultsvaryingk.xlsx
+++ b/test/resultsvaryingk.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="resultsvaryingk" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -103,6 +106,2372 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resultsvaryingk!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>new_fc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$N$2:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.10847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.199416666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.189273333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.302136666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.653653333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.492716666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.65826666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.4377</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.12893333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resultsvaryingk!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>old_fc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$O$2:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.241068666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.455608333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.681603666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.944825666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.31831</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.626593333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.10905</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.175383333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.236976666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1352540432"/>
+        <c:axId val="-1352542208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1352540432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1352542208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1352542208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1352540432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resultsvaryingk!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>new_w</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.243706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.486090666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.737926666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.996065</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.60458</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.041026666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.768559999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.035963333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.72364</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resultsvaryingk!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>old_w_kn2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$L$2:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0222053333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.045676</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0791823333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.108145666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.158607</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.201399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.274175666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.401033666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.552751333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resultsvaryingk!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>old_w_k2n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resultsvaryingk!$M$2:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.268458333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.032226666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.293173333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.21512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.600353333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.52276666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.97253333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.66916666666666</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>109.6693333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1406068672"/>
+        <c:axId val="-1434368240"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1406068672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1434368240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1434368240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1406068672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>717550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="resultsvaryingn"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="N1" t="str">
+            <v>new_fc</v>
+          </cell>
+          <cell r="O1" t="str">
+            <v>old_fc</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="I2">
+            <v>500</v>
+          </cell>
+          <cell r="N2">
+            <v>1.12016</v>
+          </cell>
+          <cell r="O2">
+            <v>0.59995766666666672</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="I3">
+            <v>1000</v>
+          </cell>
+          <cell r="N3">
+            <v>2.3225366666666667</v>
+          </cell>
+          <cell r="O3">
+            <v>2.4806766666666671</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="I4">
+            <v>1500</v>
+          </cell>
+          <cell r="N4">
+            <v>3.5360066666666667</v>
+          </cell>
+          <cell r="O4">
+            <v>11.478193333333332</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="I5">
+            <v>2000</v>
+          </cell>
+          <cell r="N5">
+            <v>4.7616233333333335</v>
+          </cell>
+          <cell r="O5">
+            <v>19.153600000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="I6">
+            <v>3000</v>
+          </cell>
+          <cell r="N6">
+            <v>7.2740900000000002</v>
+          </cell>
+          <cell r="O6">
+            <v>33.163900000000005</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="I7">
+            <v>4000</v>
+          </cell>
+          <cell r="N7">
+            <v>9.8652333333333342</v>
+          </cell>
+          <cell r="O7">
+            <v>55.419266666666665</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="I8">
+            <v>5000</v>
+          </cell>
+          <cell r="N8">
+            <v>12.814533333333335</v>
+          </cell>
+          <cell r="O8">
+            <v>70.860900000000001</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="I9">
+            <v>7500</v>
+          </cell>
+          <cell r="N9">
+            <v>19.783833333333334</v>
+          </cell>
+          <cell r="O9">
+            <v>153.63266666666667</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="I10">
+            <v>10000</v>
+          </cell>
+          <cell r="N10">
+            <v>26.63376666666667</v>
+          </cell>
+          <cell r="O10">
+            <v>264.19300000000004</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,7 +2740,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:O10"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1282,5 +3651,6 @@
   <ignoredErrors>
     <ignoredError sqref="K2" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>